<commit_message>
Phase 1 complete: AI Assisted Outreach system with cloud based follow-ups and automation
</commit_message>
<xml_diff>
--- a/data/input_excel/outreach_data.xlsx
+++ b/data/input_excel/outreach_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ai_outreach_drafter\data\input_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586B8804-AD69-4D53-8713-F042F8360234}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59B7262-055E-43E9-8217-3389643C1DD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AA8AA594-5D94-40A1-8611-A43CE59764FB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>email</t>
   </si>
@@ -61,36 +61,6 @@
   </si>
   <si>
     <t>your_skills</t>
-  </si>
-  <si>
-    <t>hr@microsoft.com</t>
-  </si>
-  <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
-    <t>Cloud Engineer</t>
-  </si>
-  <si>
-    <t>Maintain cloud systems</t>
-  </si>
-  <si>
-    <t>Netowrking, AWS, Azure, SQL</t>
-  </si>
-  <si>
-    <t>hr@IBM.com</t>
-  </si>
-  <si>
-    <t>IBM</t>
-  </si>
-  <si>
-    <t>AI Architect</t>
-  </si>
-  <si>
-    <t>create end-to-end AI systems</t>
-  </si>
-  <si>
-    <t>Machine learning, Deep learning, MLOps, Automation</t>
   </si>
 </sst>
 </file>
@@ -465,7 +435,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,46 +482,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
+      <c r="A3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
+      <c r="A4" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{6ECEC721-25B3-4D2C-9DFD-3A542D6E7193}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{6AE71536-9CF3-4984-A4A3-B49358666FA5}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{3892B1E1-EB00-4B00-9216-832AA3140664}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>